<commit_message>
20131118 fix img for category and banners
</commit_message>
<xml_diff>
--- a/contentAndGraphics/categoriesAndProducts.xlsx
+++ b/contentAndGraphics/categoriesAndProducts.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11760"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="מוצרים" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="קטגוריות" sheetId="2" r:id="rId2"/>
+    <sheet name="באנרים" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">קטגוריות!$A$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -199,12 +202,100 @@
   <si>
     <t>קומות ארוכה פרחונית</t>
   </si>
+  <si>
+    <t>מלל</t>
+  </si>
+  <si>
+    <t>חולצות בנים</t>
+  </si>
+  <si>
+    <t>חצאיות</t>
+  </si>
+  <si>
+    <t>שמלות</t>
+  </si>
+  <si>
+    <t>SALE</t>
+  </si>
+  <si>
+    <t>קטן/גדול</t>
+  </si>
+  <si>
+    <t>נושא</t>
+  </si>
+  <si>
+    <t>גדול</t>
+  </si>
+  <si>
+    <t>שני פריטים ב99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">באנר גדול עם פירסום של כל מה שיש 2 בX. </t>
+  </si>
+  <si>
+    <t>קטן</t>
+  </si>
+  <si>
+    <t>שתי שמלו ב99</t>
+  </si>
+  <si>
+    <t>מועדון לקוחות</t>
+  </si>
+  <si>
+    <t>בנות</t>
+  </si>
+  <si>
+    <t>קטגוריה</t>
+  </si>
+  <si>
+    <t>בנים</t>
+  </si>
+  <si>
+    <t>יחד עם חולצה חלקה או מקושקשת, חצאית היא הפריט האולטימטיבי.
+לבית הספר או לחגיגת יום הולדת, לארוחה אצל הסבתא או סתם אחרי צהריים בגינה - 
+החצאיות שלנו יפות ואיכותיות, עשויות בד אריג או סריג, מודפסות או חלקות.
+והעיקר - החצאיות שלנו מסתובבות !!</t>
+  </si>
+  <si>
+    <t>רמה</t>
+  </si>
+  <si>
+    <t>קטגורית אב</t>
+  </si>
+  <si>
+    <t>בית</t>
+  </si>
+  <si>
+    <t>אז מה בנים אוהבים ללבוש ? את הבגד הפשוט והנוח ביותר...
+בגדי הבנים שלנו מעוצבים ואיכותיים, הבנים יראו חגיגיים וגם יוכלו להמשיך להשתולל 
+והמחיר ? כמו תמיד אצלנו - הוגן.
+קניה מהנה !</t>
+  </si>
+  <si>
+    <t>הפכנו את כל העולם כדי להביא לכן 
+את הבגדים השמחים ביותר שמצאנו
+השתדלנו והצלחנו לשמור בשבילכן על העקרונות שלנו: איכות מצויינת, עיצוב מעודכן ומחיר הוגן
+קנייה מהנה !</t>
+  </si>
+  <si>
+    <t>פינת המציאות של שוקולדה, 
+פריטים מעונות קודמות או פריטים אחרונים מדגם.</t>
+  </si>
+  <si>
+    <t>גם גבריות וגם ילדותיות. 
+חולצות הבנים של שוקולדה מתאימות לאירועים חשובים ומשמחים - יום הולדת בגן, חתונה או ארוחה אצל סבתא</t>
+  </si>
+  <si>
+    <t>ילדות אוהבות שמלות - צבעוניות או חלקות, מבד סריג או ג'ינס
+השתדלנו שהשמלות שלנו יהיו מסתובבות, ואיפה שלא - הן "סתם" שמלות מקסימות.
+והאמת היא - גם השמלות אוהבות ילדות ...</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +315,14 @@
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -282,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -304,6 +403,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,7 +712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1208,24 +1312,218 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="99.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>2</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>2</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>2</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D1">
+    <sortState ref="A2:C7">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
+  <sortState ref="A2:D7">
+    <sortCondition ref="A2:A7"/>
+    <sortCondition ref="B2:B7"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>